<commit_message>
Add Flask app, UI, scaler, and deployment files for Heroku
</commit_message>
<xml_diff>
--- a/test_vs_prediction_results.xlsx
+++ b/test_vs_prediction_results.xlsx
@@ -462,7 +462,7 @@
         <v>4.857571407053999</v>
       </c>
       <c r="C2" t="n">
-        <v>5.234236240386963</v>
+        <v>5.315642833709717</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         <v>4.668443393714001</v>
       </c>
       <c r="C3" t="n">
-        <v>5.234839916229248</v>
+        <v>5.31564474105835</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +484,7 @@
         <v>4.80551908429409</v>
       </c>
       <c r="C4" t="n">
-        <v>5.233699321746826</v>
+        <v>5.3156418800354</v>
       </c>
     </row>
     <row r="5">
@@ -495,7 +495,7 @@
         <v>4.998026813941</v>
       </c>
       <c r="C5" t="n">
-        <v>5.234754085540771</v>
+        <v>5.315646648406982</v>
       </c>
     </row>
     <row r="6">
@@ -506,7 +506,7 @@
         <v>5.023363338918999</v>
       </c>
       <c r="C6" t="n">
-        <v>5.2377028465271</v>
+        <v>5.315648078918457</v>
       </c>
     </row>
     <row r="7">
@@ -517,7 +517,7 @@
         <v>4.822616096114</v>
       </c>
       <c r="C7" t="n">
-        <v>5.237743854522705</v>
+        <v>5.315647602081299</v>
       </c>
     </row>
     <row r="8">
@@ -528,7 +528,7 @@
         <v>4.429607166733</v>
       </c>
       <c r="C8" t="n">
-        <v>5.236936092376709</v>
+        <v>5.315646648406982</v>
       </c>
     </row>
     <row r="9">
@@ -539,7 +539,7 @@
         <v>5.438515029533001</v>
       </c>
       <c r="C9" t="n">
-        <v>5.238170146942139</v>
+        <v>5.315647602081299</v>
       </c>
     </row>
     <row r="10">
@@ -550,7 +550,7 @@
         <v>5.185118522125</v>
       </c>
       <c r="C10" t="n">
-        <v>5.237476348876953</v>
+        <v>5.315646648406982</v>
       </c>
     </row>
     <row r="11">
@@ -561,7 +561,7 @@
         <v>5.692019099825</v>
       </c>
       <c r="C11" t="n">
-        <v>5.237709522247314</v>
+        <v>5.315646648406982</v>
       </c>
     </row>
     <row r="12">
@@ -572,7 +572,7 @@
         <v>5.223532946875</v>
       </c>
       <c r="C12" t="n">
-        <v>5.237562656402588</v>
+        <v>5.315646648406982</v>
       </c>
     </row>
     <row r="13">
@@ -583,7 +583,7 @@
         <v>5.418027537625001</v>
       </c>
       <c r="C13" t="n">
-        <v>5.23716926574707</v>
+        <v>5.315649032592773</v>
       </c>
     </row>
     <row r="14">
@@ -594,7 +594,7 @@
         <v>5.840909350502</v>
       </c>
       <c r="C14" t="n">
-        <v>5.237222671508789</v>
+        <v>5.315650463104248</v>
       </c>
     </row>
     <row r="15">
@@ -605,7 +605,7 @@
         <v>5.560000497824999</v>
       </c>
       <c r="C15" t="n">
-        <v>5.236259937286377</v>
+        <v>5.315649509429932</v>
       </c>
     </row>
     <row r="16">
@@ -616,7 +616,7 @@
         <v>5.76415121375</v>
       </c>
       <c r="C16" t="n">
-        <v>5.23651647567749</v>
+        <v>5.315650463104248</v>
       </c>
     </row>
     <row r="17">
@@ -627,7 +627,7 @@
         <v>5.407662430525001</v>
       </c>
       <c r="C17" t="n">
-        <v>5.236937046051025</v>
+        <v>5.315648555755615</v>
       </c>
     </row>
     <row r="18">
@@ -638,7 +638,7 @@
         <v>5.635396825932</v>
       </c>
       <c r="C18" t="n">
-        <v>5.237905025482178</v>
+        <v>5.315648555755615</v>
       </c>
     </row>
     <row r="19">
@@ -649,7 +649,7 @@
         <v>5.904906289082</v>
       </c>
       <c r="C19" t="n">
-        <v>5.237595081329346</v>
+        <v>5.315650463104248</v>
       </c>
     </row>
     <row r="20">
@@ -660,7 +660,7 @@
         <v>5.754983475486</v>
       </c>
       <c r="C20" t="n">
-        <v>5.237764835357666</v>
+        <v>5.315648555755615</v>
       </c>
     </row>
     <row r="21">
@@ -671,7 +671,7 @@
         <v>6.125426000894999</v>
       </c>
       <c r="C21" t="n">
-        <v>5.23836088180542</v>
+        <v>5.315647602081299</v>
       </c>
     </row>
     <row r="22">
@@ -682,7 +682,7 @@
         <v>5.406917101506</v>
       </c>
       <c r="C22" t="n">
-        <v>5.237873077392578</v>
+        <v>5.315646648406982</v>
       </c>
     </row>
     <row r="23">
@@ -693,7 +693,7 @@
         <v>6.574890841338999</v>
       </c>
       <c r="C23" t="n">
-        <v>5.237945556640625</v>
+        <v>5.315648555755615</v>
       </c>
     </row>
     <row r="24">
@@ -704,7 +704,7 @@
         <v>6.405723786886</v>
       </c>
       <c r="C24" t="n">
-        <v>5.237551212310791</v>
+        <v>5.315650463104248</v>
       </c>
     </row>
     <row r="25">
@@ -715,7 +715,7 @@
         <v>6.718604456511001</v>
       </c>
       <c r="C25" t="n">
-        <v>5.23773193359375</v>
+        <v>5.315648555755615</v>
       </c>
     </row>
     <row r="26">
@@ -726,7 +726,7 @@
         <v>6.05485169882</v>
       </c>
       <c r="C26" t="n">
-        <v>5.237066745758057</v>
+        <v>5.31564998626709</v>
       </c>
     </row>
     <row r="27">
@@ -737,7 +737,7 @@
         <v>5.72217794552</v>
       </c>
       <c r="C27" t="n">
-        <v>5.23717737197876</v>
+        <v>5.315650463104248</v>
       </c>
     </row>
     <row r="28">
@@ -748,7 +748,7 @@
         <v>6.699475908175</v>
       </c>
       <c r="C28" t="n">
-        <v>5.237288951873779</v>
+        <v>5.315651416778564</v>
       </c>
     </row>
     <row r="29">
@@ -759,7 +759,7 @@
         <v>5.647809795596</v>
       </c>
       <c r="C29" t="n">
-        <v>5.237312316894531</v>
+        <v>5.315650463104248</v>
       </c>
     </row>
     <row r="30">
@@ -770,7 +770,7 @@
         <v>5.854452414233</v>
       </c>
       <c r="C30" t="n">
-        <v>5.237972259521484</v>
+        <v>5.315651416778564</v>
       </c>
     </row>
     <row r="31">
@@ -781,7 +781,7 @@
         <v>5.460436904519</v>
       </c>
       <c r="C31" t="n">
-        <v>5.237992763519287</v>
+        <v>5.315651416778564</v>
       </c>
     </row>
     <row r="32">
@@ -792,7 +792,7 @@
         <v>5.755830683622917</v>
       </c>
       <c r="C32" t="n">
-        <v>5.237462043762207</v>
+        <v>5.315652370452881</v>
       </c>
     </row>
     <row r="33">
@@ -803,7 +803,7 @@
         <v>5.991571160172917</v>
       </c>
       <c r="C33" t="n">
-        <v>5.238211154937744</v>
+        <v>5.315651893615723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add time features and retrain Random Forest/XGBoost models. Ready for deployment.
</commit_message>
<xml_diff>
--- a/test_vs_prediction_results.xlsx
+++ b/test_vs_prediction_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,354 +456,343 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44774</v>
+        <v>44805</v>
       </c>
       <c r="B2" t="n">
-        <v>4.857571407053999</v>
+        <v>4.668443393714001</v>
       </c>
       <c r="C2" t="n">
-        <v>5.315642833709717</v>
+        <v>5.263088226318359</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44805</v>
+        <v>44835</v>
       </c>
       <c r="B3" t="n">
-        <v>4.668443393714001</v>
+        <v>4.80551908429409</v>
       </c>
       <c r="C3" t="n">
-        <v>5.31564474105835</v>
+        <v>5.263363838195801</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="B4" t="n">
-        <v>4.80551908429409</v>
+        <v>4.998026813941</v>
       </c>
       <c r="C4" t="n">
-        <v>5.3156418800354</v>
+        <v>5.263692855834961</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44866</v>
+        <v>44896</v>
       </c>
       <c r="B5" t="n">
-        <v>4.998026813941</v>
+        <v>5.023363338918999</v>
       </c>
       <c r="C5" t="n">
-        <v>5.315646648406982</v>
+        <v>5.264224529266357</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44896</v>
+        <v>44927</v>
       </c>
       <c r="B6" t="n">
-        <v>5.023363338918999</v>
+        <v>4.822616096114</v>
       </c>
       <c r="C6" t="n">
-        <v>5.315648078918457</v>
+        <v>5.26333475112915</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="B7" t="n">
-        <v>4.822616096114</v>
+        <v>4.429607166733</v>
       </c>
       <c r="C7" t="n">
-        <v>5.315647602081299</v>
+        <v>5.262760639190674</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="B8" t="n">
-        <v>4.429607166733</v>
+        <v>5.438515029533001</v>
       </c>
       <c r="C8" t="n">
-        <v>5.315646648406982</v>
+        <v>5.263341903686523</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="B9" t="n">
-        <v>5.438515029533001</v>
+        <v>5.185118522125</v>
       </c>
       <c r="C9" t="n">
-        <v>5.315647602081299</v>
+        <v>5.262135982513428</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="B10" t="n">
-        <v>5.185118522125</v>
+        <v>5.692019099825</v>
       </c>
       <c r="C10" t="n">
-        <v>5.315646648406982</v>
+        <v>5.26285982131958</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="B11" t="n">
-        <v>5.692019099825</v>
+        <v>5.223532946875</v>
       </c>
       <c r="C11" t="n">
-        <v>5.315646648406982</v>
+        <v>5.262763500213623</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45078</v>
+        <v>45108</v>
       </c>
       <c r="B12" t="n">
-        <v>5.223532946875</v>
+        <v>5.418027537625001</v>
       </c>
       <c r="C12" t="n">
-        <v>5.315646648406982</v>
+        <v>5.26339054107666</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45108</v>
+        <v>45139</v>
       </c>
       <c r="B13" t="n">
-        <v>5.418027537625001</v>
+        <v>5.840909350502</v>
       </c>
       <c r="C13" t="n">
-        <v>5.315649032592773</v>
+        <v>5.26413106918335</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45139</v>
+        <v>45170</v>
       </c>
       <c r="B14" t="n">
-        <v>5.840909350502</v>
+        <v>5.560000497824999</v>
       </c>
       <c r="C14" t="n">
-        <v>5.315650463104248</v>
+        <v>5.264116764068604</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="B15" t="n">
-        <v>5.560000497824999</v>
+        <v>5.76415121375</v>
       </c>
       <c r="C15" t="n">
-        <v>5.315649509429932</v>
+        <v>5.264317035675049</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="B16" t="n">
-        <v>5.76415121375</v>
+        <v>5.407662430525001</v>
       </c>
       <c r="C16" t="n">
-        <v>5.315650463104248</v>
+        <v>5.264308452606201</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="B17" t="n">
-        <v>5.407662430525001</v>
+        <v>5.635396825932</v>
       </c>
       <c r="C17" t="n">
-        <v>5.315648555755615</v>
+        <v>5.263980388641357</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="B18" t="n">
-        <v>5.635396825932</v>
+        <v>5.904906289082</v>
       </c>
       <c r="C18" t="n">
-        <v>5.315648555755615</v>
+        <v>5.26328706741333</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45292</v>
+        <v>45323</v>
       </c>
       <c r="B19" t="n">
-        <v>5.904906289082</v>
+        <v>5.754983475486</v>
       </c>
       <c r="C19" t="n">
-        <v>5.315650463104248</v>
+        <v>5.262651443481445</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45323</v>
+        <v>45352</v>
       </c>
       <c r="B20" t="n">
-        <v>5.754983475486</v>
+        <v>6.125426000894999</v>
       </c>
       <c r="C20" t="n">
-        <v>5.315648555755615</v>
+        <v>5.26248025894165</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45352</v>
+        <v>45383</v>
       </c>
       <c r="B21" t="n">
-        <v>6.125426000894999</v>
+        <v>5.406917101506</v>
       </c>
       <c r="C21" t="n">
-        <v>5.315647602081299</v>
+        <v>5.260635852813721</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="B22" t="n">
-        <v>5.406917101506</v>
+        <v>6.574890841338999</v>
       </c>
       <c r="C22" t="n">
-        <v>5.315646648406982</v>
+        <v>5.261858463287354</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="B23" t="n">
-        <v>6.574890841338999</v>
+        <v>6.405723786886</v>
       </c>
       <c r="C23" t="n">
-        <v>5.315648555755615</v>
+        <v>5.262577056884766</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="B24" t="n">
-        <v>6.405723786886</v>
+        <v>6.718604456511001</v>
       </c>
       <c r="C24" t="n">
-        <v>5.315650463104248</v>
+        <v>5.263165950775146</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45474</v>
+        <v>45505</v>
       </c>
       <c r="B25" t="n">
-        <v>6.718604456511001</v>
+        <v>6.05485169882</v>
       </c>
       <c r="C25" t="n">
-        <v>5.315648555755615</v>
+        <v>5.263201236724854</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="B26" t="n">
-        <v>6.05485169882</v>
+        <v>5.72217794552</v>
       </c>
       <c r="C26" t="n">
-        <v>5.31564998626709</v>
+        <v>5.263431072235107</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="B27" t="n">
-        <v>5.72217794552</v>
+        <v>6.699475908175</v>
       </c>
       <c r="C27" t="n">
-        <v>5.315650463104248</v>
+        <v>5.263772964477539</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="B28" t="n">
-        <v>6.699475908175</v>
+        <v>5.647809795596</v>
       </c>
       <c r="C28" t="n">
-        <v>5.315651416778564</v>
+        <v>5.263920307159424</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="B29" t="n">
-        <v>5.647809795596</v>
+        <v>5.854452414233</v>
       </c>
       <c r="C29" t="n">
-        <v>5.315650463104248</v>
+        <v>5.263461589813232</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="B30" t="n">
-        <v>5.854452414233</v>
+        <v>5.460436904519</v>
       </c>
       <c r="C30" t="n">
-        <v>5.315651416778564</v>
+        <v>5.262987613677979</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45658</v>
+        <v>45689</v>
       </c>
       <c r="B31" t="n">
-        <v>5.460436904519</v>
+        <v>5.755830683622917</v>
       </c>
       <c r="C31" t="n">
-        <v>5.315651416778564</v>
+        <v>5.262224674224854</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45689</v>
+        <v>45717</v>
       </c>
       <c r="B32" t="n">
-        <v>5.755830683622917</v>
+        <v>5.991571160172917</v>
       </c>
       <c r="C32" t="n">
-        <v>5.315652370452881</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>45717</v>
-      </c>
-      <c r="B33" t="n">
-        <v>5.991571160172917</v>
-      </c>
-      <c r="C33" t="n">
-        <v>5.315651893615723</v>
+        <v>5.262828350067139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>